<commit_message>
PuLP and Pyhton MIP Tutorial Updated
</commit_message>
<xml_diff>
--- a/docs/source/MIP/tutorials/dataset/Demands.xlsx
+++ b/docs/source/MIP/tutorials/dataset/Demands.xlsx
@@ -1,28 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ffraile\PycharmProjects\operations-research-notebooks\docs\source\MIP\tutorials\dataset\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C7E0DE-45B4-4198-A7F3-350453ECC470}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="23895" windowHeight="14535"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="23895" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" r:id="rId1" name="Demands"/>
+    <sheet name="Demands" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Demands">'Demands'!$A$1:$C$19</definedName>
+    <definedName name="Demands">Demands!$A$1:$C$19</definedName>
   </definedNames>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>IdRegion</t>
+  </si>
+  <si>
+    <t>IdProduct</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="MS Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -55,11 +75,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -101,7 +129,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,9 +161,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -167,6 +213,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -342,227 +406,221 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row outlineLevel="0" r="1">
-      <c r="A1" s="0" t="inlineStr">
-        <is>
-          <t>IdRegion</t>
-        </is>
-      </c>
-      <c r="B1" s="0" t="inlineStr">
-        <is>
-          <t>IdProduct</t>
-        </is>
-      </c>
-      <c r="C1" s="0" t="inlineStr">
-        <is>
-          <t>Demand</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0">
-        <v>1</v>
-      </c>
-      <c r="C2" s="0">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>654</v>
       </c>
     </row>
-    <row outlineLevel="0" r="3">
-      <c r="A3" s="0">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0">
-        <v>2</v>
-      </c>
-      <c r="C3" s="0">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
         <v>535</v>
       </c>
     </row>
-    <row outlineLevel="0" r="4">
-      <c r="A4" s="0">
-        <v>1</v>
-      </c>
-      <c r="B4" s="0">
-        <v>3</v>
-      </c>
-      <c r="C4" s="0">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
         <v>588</v>
       </c>
     </row>
-    <row outlineLevel="0" r="5">
-      <c r="A5" s="0">
-        <v>2</v>
-      </c>
-      <c r="B5" s="0">
-        <v>1</v>
-      </c>
-      <c r="C5" s="0">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
         <v>636</v>
       </c>
     </row>
-    <row outlineLevel="0" r="6">
-      <c r="A6" s="0">
-        <v>2</v>
-      </c>
-      <c r="B6" s="0">
-        <v>2</v>
-      </c>
-      <c r="C6" s="0">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
         <v>869</v>
       </c>
     </row>
-    <row outlineLevel="0" r="7">
-      <c r="A7" s="0">
-        <v>2</v>
-      </c>
-      <c r="B7" s="0">
-        <v>3</v>
-      </c>
-      <c r="C7" s="0">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
         <v>656</v>
       </c>
     </row>
-    <row outlineLevel="0" r="8">
-      <c r="A8" s="0">
-        <v>3</v>
-      </c>
-      <c r="B8" s="0">
-        <v>1</v>
-      </c>
-      <c r="C8" s="0">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
         <v>683</v>
       </c>
     </row>
-    <row outlineLevel="0" r="9">
-      <c r="A9" s="0">
-        <v>3</v>
-      </c>
-      <c r="B9" s="0">
-        <v>2</v>
-      </c>
-      <c r="C9" s="0">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
         <v>966</v>
       </c>
     </row>
-    <row outlineLevel="0" r="10">
-      <c r="A10" s="0">
-        <v>3</v>
-      </c>
-      <c r="B10" s="0">
-        <v>3</v>
-      </c>
-      <c r="C10" s="0">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
         <v>665</v>
       </c>
     </row>
-    <row outlineLevel="0" r="11">
-      <c r="A11" s="0">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>4</v>
       </c>
-      <c r="B11" s="0">
-        <v>1</v>
-      </c>
-      <c r="C11" s="0">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
         <v>911</v>
       </c>
     </row>
-    <row outlineLevel="0" r="12">
-      <c r="A12" s="0">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>4</v>
       </c>
-      <c r="B12" s="0">
-        <v>2</v>
-      </c>
-      <c r="C12" s="0">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
         <v>646</v>
       </c>
     </row>
-    <row outlineLevel="0" r="13">
-      <c r="A13" s="0">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>4</v>
       </c>
-      <c r="B13" s="0">
-        <v>3</v>
-      </c>
-      <c r="C13" s="0">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
         <v>863</v>
       </c>
     </row>
-    <row outlineLevel="0" r="14">
-      <c r="A14" s="0">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>5</v>
       </c>
-      <c r="B14" s="0">
-        <v>1</v>
-      </c>
-      <c r="C14" s="0">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
         <v>605</v>
       </c>
     </row>
-    <row outlineLevel="0" r="15">
-      <c r="A15" s="0">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>5</v>
       </c>
-      <c r="B15" s="0">
-        <v>2</v>
-      </c>
-      <c r="C15" s="0">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
         <v>804</v>
       </c>
     </row>
-    <row outlineLevel="0" r="16">
-      <c r="A16" s="0">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>5</v>
       </c>
-      <c r="B16" s="0">
-        <v>3</v>
-      </c>
-      <c r="C16" s="0">
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
         <v>633</v>
       </c>
     </row>
-    <row outlineLevel="0" r="17">
-      <c r="A17" s="0">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>6</v>
       </c>
-      <c r="B17" s="0">
-        <v>1</v>
-      </c>
-      <c r="C17" s="0">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
         <v>613</v>
       </c>
     </row>
-    <row outlineLevel="0" r="18">
-      <c r="A18" s="0">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>6</v>
       </c>
-      <c r="B18" s="0">
-        <v>2</v>
-      </c>
-      <c r="C18" s="0">
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
         <v>892</v>
       </c>
     </row>
-    <row outlineLevel="0" r="19">
-      <c r="A19" s="0">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>6</v>
       </c>
-      <c r="B19" s="0">
-        <v>3</v>
-      </c>
-      <c r="C19" s="0">
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
         <v>651</v>
       </c>
     </row>

</xml_diff>